<commit_message>
Result analysis per class and exported into Excel sheet
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,9 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
   <si>
     <t>First class</t>
+  </si>
+  <si>
+    <t>First class With Distinction</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -374,44 +380,193 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:7">
       <c r="A1" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>75</v>
+      </c>
+      <c r="C2">
+        <v>88</v>
+      </c>
+      <c r="D2">
+        <v>74</v>
+      </c>
+      <c r="E2">
+        <v>238</v>
+      </c>
+      <c r="F2">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>85</v>
+      </c>
+      <c r="C3">
+        <v>90</v>
+      </c>
+      <c r="D3">
+        <v>69</v>
+      </c>
+      <c r="E3">
+        <v>246</v>
+      </c>
+      <c r="F3">
+        <v>82</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>65</v>
+      </c>
+      <c r="C4">
+        <v>78</v>
+      </c>
+      <c r="D4">
+        <v>99</v>
+      </c>
+      <c r="E4">
+        <v>245</v>
+      </c>
+      <c r="F4">
+        <v>81</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>92</v>
+      </c>
+      <c r="C5">
+        <v>74</v>
+      </c>
+      <c r="D5">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>215</v>
+      </c>
+      <c r="F5">
+        <v>71</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>75</v>
+      </c>
+      <c r="C6">
+        <v>96</v>
+      </c>
+      <c r="D6">
+        <v>74</v>
+      </c>
+      <c r="E6">
+        <v>250</v>
+      </c>
+      <c r="F6">
+        <v>83</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>55</v>
+      </c>
+      <c r="C7">
+        <v>47</v>
+      </c>
+      <c r="D7">
+        <v>36</v>
+      </c>
+      <c r="E7">
+        <v>144</v>
+      </c>
+      <c r="F7">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
+      <c r="C8">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
+      <c r="D8">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="E8">
+        <v>207</v>
+      </c>
+      <c r="F8">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>